<commit_message>
Update manual annotation, import bioqc results.
</commit_message>
<xml_diff>
--- a/manual_annotation/signature_sets.xlsx
+++ b/manual_annotation/signature_sets.xlsx
@@ -4,29 +4,30 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20115" windowHeight="7740" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="165" windowWidth="20115" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="bioqc_solid" sheetId="1" r:id="rId1"/>
     <sheet name="gtex_solid" sheetId="4" r:id="rId2"/>
-    <sheet name="pivot" sheetId="3" r:id="rId3"/>
+    <sheet name="gtex_all" sheetId="5" r:id="rId3"/>
+    <sheet name="pivot" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="all_tissues">[1]all_tissues.dbexport!$C:$C</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="221">
   <si>
     <t>Adipose_NGS_RNASEQATLAS_0.6_3</t>
   </si>
@@ -665,6 +666,30 @@
   </si>
   <si>
     <t>gtex_ngs_0.85_5.gmt</t>
+  </si>
+  <si>
+    <t>adrenal gland</t>
+  </si>
+  <si>
+    <t>salivary gland</t>
+  </si>
+  <si>
+    <t>stomach</t>
+  </si>
+  <si>
+    <t>testis</t>
+  </si>
+  <si>
+    <t>uterus</t>
+  </si>
+  <si>
+    <t>jejunum</t>
+  </si>
+  <si>
+    <t>vagina</t>
+  </si>
+  <si>
+    <t>vulva</t>
   </si>
 </sst>
 </file>
@@ -1660,6 +1685,11 @@
             <v>adipose</v>
           </cell>
         </row>
+        <row r="238">
+          <cell r="C238" t="str">
+            <v>colon</v>
+          </cell>
+        </row>
         <row r="243">
           <cell r="C243" t="str">
             <v>skin</v>
@@ -1743,6 +1773,61 @@
         <row r="445">
           <cell r="C445" t="str">
             <v>skin</v>
+          </cell>
+        </row>
+        <row r="555">
+          <cell r="C555" t="str">
+            <v>colon</v>
+          </cell>
+        </row>
+        <row r="656">
+          <cell r="C656" t="str">
+            <v>jejunum</v>
+          </cell>
+        </row>
+        <row r="1320">
+          <cell r="C1320" t="str">
+            <v>adrenal gland</v>
+          </cell>
+        </row>
+        <row r="4056">
+          <cell r="C4056" t="str">
+            <v>skeletal muscle</v>
+          </cell>
+        </row>
+        <row r="4566">
+          <cell r="C4566" t="str">
+            <v>adrenal gland</v>
+          </cell>
+        </row>
+        <row r="4780">
+          <cell r="C4780" t="str">
+            <v>adrenal gland</v>
+          </cell>
+        </row>
+        <row r="4805">
+          <cell r="C4805" t="str">
+            <v>uterus</v>
+          </cell>
+        </row>
+        <row r="4812">
+          <cell r="C4812" t="str">
+            <v>adrenal gland</v>
+          </cell>
+        </row>
+        <row r="4995">
+          <cell r="C4995" t="str">
+            <v>uterus</v>
+          </cell>
+        </row>
+        <row r="5158">
+          <cell r="C5158" t="str">
+            <v>uterus</v>
+          </cell>
+        </row>
+        <row r="7432">
+          <cell r="C7432" t="str">
+            <v>uterus</v>
           </cell>
         </row>
       </sheetData>
@@ -3234,8 +3319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3537,6 +3622,9 @@
       <c r="B25" t="s">
         <v>211</v>
       </c>
+      <c r="C25" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -4193,7 +4281,7 @@
         <v>211</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
       <c r="D78" t="s">
         <v>173</v>
@@ -4844,6 +4932,9 @@
       <c r="B134" t="s">
         <v>211</v>
       </c>
+      <c r="C134" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
@@ -4852,6 +4943,9 @@
       <c r="B135" t="s">
         <v>211</v>
       </c>
+      <c r="C135" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
@@ -4860,6 +4954,9 @@
       <c r="B136" t="s">
         <v>211</v>
       </c>
+      <c r="C136" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -4868,6 +4965,9 @@
       <c r="B137" t="s">
         <v>211</v>
       </c>
+      <c r="C137" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -4876,6 +4976,9 @@
       <c r="B138" t="s">
         <v>211</v>
       </c>
+      <c r="C138" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -4884,6 +4987,9 @@
       <c r="B139" t="s">
         <v>211</v>
       </c>
+      <c r="C139" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
@@ -4892,6 +4998,9 @@
       <c r="B140" t="s">
         <v>211</v>
       </c>
+      <c r="C140" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
@@ -4900,6 +5009,9 @@
       <c r="B141" t="s">
         <v>211</v>
       </c>
+      <c r="C141" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
@@ -4908,6 +5020,9 @@
       <c r="B142" t="s">
         <v>211</v>
       </c>
+      <c r="C142" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
@@ -4925,7 +5040,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>160</v>
       </c>
@@ -4933,7 +5048,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>161</v>
       </c>
@@ -4941,7 +5056,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>162</v>
       </c>
@@ -4949,7 +5064,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>163</v>
       </c>
@@ -4957,7 +5072,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>164</v>
       </c>
@@ -4965,7 +5080,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>165</v>
       </c>
@@ -4973,52 +5088,70 @@
         <v>211</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>166</v>
       </c>
       <c r="B151" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C151" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>167</v>
       </c>
       <c r="B152" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>168</v>
       </c>
       <c r="B153" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C153" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>169</v>
       </c>
       <c r="B154" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C154" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>170</v>
       </c>
       <c r="B155" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C155" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>171</v>
       </c>
       <c r="B156" t="s">
         <v>211</v>
+      </c>
+      <c r="C156" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -5035,7 +5168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -5349,6 +5482,383 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>203</v>
+      </c>
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>204</v>
+      </c>
+      <c r="B23" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C24" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>206</v>
+      </c>
+      <c r="B25" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B23"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updating views for new db scheme.
</commit_message>
<xml_diff>
--- a/manual_annotation/signature_sets.xlsx
+++ b/manual_annotation/signature_sets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="165" windowWidth="20115" windowHeight="7680"/>
+    <workbookView xWindow="120" yWindow="165" windowWidth="20115" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="bioqc_solid" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
-    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="221">
   <si>
     <t>Adipose_NGS_RNASEQATLAS_0.6_3</t>
   </si>
@@ -1838,44 +1838,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Sturm, Gregor" refreshedDate="42704.57436608796" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="156">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="C1:C1048576" sheet="bioqc_solid"/>
-  </cacheSource>
-  <cacheFields count="1">
-    <cacheField name="tissue" numFmtId="0">
-      <sharedItems containsBlank="1" count="18">
-        <s v="adipose"/>
-        <m/>
-        <s v="brain"/>
-        <s v="breast"/>
-        <s v="colon"/>
-        <s v="heart"/>
-        <s v="kidney"/>
-        <s v="liver"/>
-        <s v="lung"/>
-        <s v="ovary"/>
-        <s v="prostate"/>
-        <s v="skeletal muscle"/>
-        <s v="spleen"/>
-        <s v="blood"/>
-        <s v="bone marrow"/>
-        <s v="skin"/>
-        <s v="pancreas"/>
-        <s v="placenta"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Sturm, Gregor" refreshedDate="42704.576775925925" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="156">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Sturm, Gregor" refreshedDate="42709.550174305557" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="144">
   <cacheSource type="worksheet">
     <worksheetSource ref="D1:D1048576" sheet="bioqc_solid"/>
   </cacheSource>
@@ -1906,13 +1869,63 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Sturm, Gregor" refreshedDate="42709.550194675925" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="156">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="C1:C1048576" sheet="bioqc_solid"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="tissue" numFmtId="0">
+      <sharedItems containsBlank="1" count="25">
+        <s v="adipose"/>
+        <m/>
+        <s v="brain"/>
+        <s v="breast"/>
+        <s v="colon"/>
+        <s v="heart"/>
+        <s v="kidney"/>
+        <s v="liver"/>
+        <s v="lung"/>
+        <s v="ovary"/>
+        <s v="prostate"/>
+        <s v="skeletal muscle"/>
+        <s v="spleen"/>
+        <s v="blood"/>
+        <s v="adrenal gland"/>
+        <s v="bone marrow"/>
+        <s v="skin"/>
+        <s v="jejunum"/>
+        <s v="pancreas"/>
+        <s v="placenta"/>
+        <s v="stomach"/>
+        <s v="testis"/>
+        <s v="uterus"/>
+        <s v="vagina"/>
+        <s v="vulva"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="156">
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="144">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -1921,460 +1934,418 @@
     <x v="3"/>
   </r>
   <r>
+    <x v="1"/>
+  </r>
+  <r>
     <x v="4"/>
   </r>
   <r>
     <x v="5"/>
   </r>
   <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
     <x v="2"/>
   </r>
   <r>
-    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
   </r>
   <r>
     <x v="7"/>
   </r>
   <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
     <x v="8"/>
   </r>
   <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -2385,13 +2356,7 @@
     <x v="0"/>
   </r>
   <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="2"/>
@@ -2400,460 +2365,466 @@
     <x v="3"/>
   </r>
   <r>
-    <x v="1"/>
-  </r>
-  <r>
     <x v="4"/>
   </r>
   <r>
     <x v="5"/>
   </r>
   <r>
+    <x v="2"/>
+  </r>
+  <r>
     <x v="6"/>
   </r>
   <r>
-    <x v="0"/>
-  </r>
-  <r>
     <x v="7"/>
   </r>
   <r>
     <x v="8"/>
   </r>
   <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
     <x v="3"/>
   </r>
   <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
   </r>
   <r>
     <x v="9"/>
   </r>
   <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
   </r>
   <r>
     <x v="2"/>
   </r>
   <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B4:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" showAll="0">
@@ -2929,14 +2900,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:A23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:A30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" showAll="0">
-      <items count="19">
+      <items count="26">
         <item x="0"/>
         <item x="13"/>
-        <item x="14"/>
+        <item x="15"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
@@ -2945,13 +2916,20 @@
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
-        <item x="16"/>
-        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
         <item x="10"/>
         <item x="11"/>
-        <item x="15"/>
+        <item x="16"/>
         <item x="12"/>
         <item x="1"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2959,7 +2937,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="19">
+  <rowItems count="26">
     <i>
       <x/>
     </i>
@@ -3013,6 +2991,27 @@
     </i>
     <i>
       <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
     </i>
     <i t="grand">
       <x/>
@@ -3319,8 +3318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5169,7 +5168,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5415,7 +5414,7 @@
         <v>212</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
       <c r="D22" t="s">
         <v>173</v>
@@ -5485,8 +5484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5774,7 +5773,7 @@
         <v>212</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
       <c r="D22" t="s">
         <v>173</v>
@@ -5860,10 +5859,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B23"/>
+  <dimension ref="A3:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6016,6 +6015,41 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add BioQC to makefile including some bugfixes.
</commit_message>
<xml_diff>
--- a/manual_annotation/signature_sets.xlsx
+++ b/manual_annotation/signature_sets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="165" windowWidth="20115" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="225" windowWidth="20115" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="bioqc_solid" sheetId="1" r:id="rId1"/>
@@ -27,98 +27,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="221">
-  <si>
-    <t>Adipose_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="253">
   <si>
     <t>adipose</t>
   </si>
   <si>
-    <t>Adrenal_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
-    <t>Brain_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>brain</t>
   </si>
   <si>
-    <t>Breast_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>breast</t>
   </si>
   <si>
-    <t>Colon_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>colon</t>
   </si>
   <si>
-    <t>Heart_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>heart</t>
   </si>
   <si>
-    <t>Hypothalamus_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
-    <t>Kidney_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>kidney</t>
   </si>
   <si>
-    <t>Liver_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>liver</t>
   </si>
   <si>
-    <t>Lung_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>lung</t>
   </si>
   <si>
-    <t>Lymph_node_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
-    <t>Ovary_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>ovary</t>
   </si>
   <si>
-    <t>Prostate_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>prostate</t>
   </si>
   <si>
-    <t>Skeletal_Muscle_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>skeletal muscle</t>
   </si>
   <si>
-    <t>Spleen_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>spleen</t>
   </si>
   <si>
-    <t>Testis_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
-    <t>Thyroid_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
-    <t>WBC_NGS_RNASEQATLAS_0.6_3</t>
-  </si>
-  <si>
     <t>blood</t>
   </si>
   <si>
@@ -140,9 +86,6 @@
     <t>Adrenal_Gland_NR_0.7_3</t>
   </si>
   <si>
-    <t>Artery_coronary_NR_0.7_3</t>
-  </si>
-  <si>
     <t>Blood_NR_0.7_3</t>
   </si>
   <si>
@@ -398,9 +341,6 @@
     <t>Muscle_cardiac_ventricle_NR_0.7_3</t>
   </si>
   <si>
-    <t>Muscle_skeletal_NR_0.7_3</t>
-  </si>
-  <si>
     <t>Muscle_skeletal_tongue_NR_0.7_3</t>
   </si>
   <si>
@@ -690,6 +630,162 @@
   </si>
   <si>
     <t>vulva</t>
+  </si>
+  <si>
+    <t>Brain_Putamen_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_Spinal_cord_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Heart_Atrial_Appendage_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Heart_Left_Ventricle_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_Substantia_nigra_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Intestine_Colon_cecum_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_basal_ganglia_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_frontal_lobe_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_occipital_lobe_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Kidney_Cortex_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_stem_Tegmental_area_v_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_stem_vest_nuclei_s_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Breast_Mammary_Tissue_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Adipose_Subcutaneous_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Adipose_Visceral_Omentum_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Colon_Transverse_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Artery_Aorta_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Artery_Coronary_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Artery_Tibial_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_Anterior_cingulate_cortex_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Esophagus_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_Cerebellar_Hemisphere_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Esophagus_Mucosa_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Esophagus_Muscularis_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_Corpus_callosum_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Fallopian_Tube_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Fibroblast_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_Frontal_Cortex_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Brain_Midbrain_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Muscle_Skeletal_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Monocyte, intermediate_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Monocyte, non-classical_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Monocyte_Linsley_0.7_3</t>
+  </si>
+  <si>
+    <t>Monocyte_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>NK cells_Linsley_0.7_3</t>
+  </si>
+  <si>
+    <t>NK cells_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Neutrophil granulocyte_Linsley_0.7_3</t>
+  </si>
+  <si>
+    <t>Erythrocyte_sig_top50_corr_HBA1_in_Blood</t>
+  </si>
+  <si>
+    <t>Nerve_Tibial_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocytes_NR_0.7_3</t>
+  </si>
+  <si>
+    <t>Blood_Linsley_0.7_3</t>
+  </si>
+  <si>
+    <t>Dendritic cell_myeloid_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Dendritic cell_plasmacytoid_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocyte B_Linsley_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocyte B_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocyte T, CD4 PB_Linsley_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocyte T, CD4+ CD8dim_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocyte T, CD8 PB_Linsley_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocyte T, CD8 PB_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocyte T, Regulatory_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>Lymphocyte T, helper_Roche_0.7_3</t>
+  </si>
+  <si>
+    <t>nerve</t>
   </si>
 </sst>
 </file>
@@ -1174,13 +1270,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3316,10 +3413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D156"/>
+  <dimension ref="A1:J187"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3327,324 +3424,328 @@
     <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>172</v>
+        <v>191</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+        <v>191</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>173</v>
+        <v>191</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>174</v>
+        <v>191</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>217</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>211</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>219</v>
       </c>
       <c r="B12" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>241</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>220</v>
       </c>
       <c r="B18" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
+      <c r="D20" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
+      <c r="D21" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
       </c>
+      <c r="D22" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>225</v>
       </c>
       <c r="B24" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C25" t="s">
-        <v>213</v>
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3652,1514 +3753,1827 @@
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="B29" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>208</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>229</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>209</v>
       </c>
       <c r="B37" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>201</v>
       </c>
       <c r="B40" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>202</v>
       </c>
       <c r="B41" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>211</v>
       </c>
       <c r="B44" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="B45" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>205</v>
       </c>
       <c r="B47" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="B51" t="s">
-        <v>211</v>
-      </c>
-      <c r="C51" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>216</v>
       </c>
       <c r="B54" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C54" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>30</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>211</v>
-      </c>
-      <c r="C55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D55" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>242</v>
       </c>
       <c r="B56" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>243</v>
       </c>
       <c r="B57" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C57" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D57" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B60" t="s">
-        <v>211</v>
-      </c>
-      <c r="C60" t="s">
-        <v>73</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>12</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>211</v>
-      </c>
-      <c r="C63" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D64" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C65" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>211</v>
-      </c>
-      <c r="C66" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
-      </c>
-      <c r="C67" t="s">
-        <v>30</v>
-      </c>
-      <c r="D67" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>238</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C69" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D69" t="s">
-        <v>172</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C70" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D70" t="s">
-        <v>172</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
-      </c>
-      <c r="C71" t="s">
-        <v>4</v>
-      </c>
-      <c r="D71" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
-      </c>
-      <c r="C72" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>221</v>
       </c>
       <c r="B73" t="s">
-        <v>211</v>
-      </c>
-      <c r="C73" t="s">
-        <v>30</v>
-      </c>
-      <c r="D73" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
-      </c>
-      <c r="C74" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>226</v>
       </c>
       <c r="B75" t="s">
-        <v>211</v>
-      </c>
-      <c r="C75" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>227</v>
       </c>
       <c r="B76" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B77" t="s">
-        <v>211</v>
-      </c>
-      <c r="C77" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B78" t="s">
-        <v>211</v>
-      </c>
-      <c r="C78" t="s">
-        <v>218</v>
-      </c>
-      <c r="D78" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="B79" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>211</v>
-      </c>
-      <c r="C80" t="s">
-        <v>13</v>
-      </c>
-      <c r="D80" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B81" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="B82" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C82" t="s">
-        <v>13</v>
-      </c>
-      <c r="D82" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>203</v>
       </c>
       <c r="B83" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>204</v>
       </c>
       <c r="B84" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="B85" t="s">
-        <v>211</v>
-      </c>
-      <c r="C85" t="s">
-        <v>15</v>
-      </c>
-      <c r="D85" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
-        <v>211</v>
-      </c>
-      <c r="C86" t="s">
-        <v>15</v>
-      </c>
-      <c r="D86" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="B87" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C87" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="D87" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="B88" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C88" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="B89" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C89" t="s">
+        <v>198</v>
+      </c>
+      <c r="D89" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="B90" t="s">
-        <v>211</v>
-      </c>
-      <c r="C90" t="s">
-        <v>30</v>
-      </c>
-      <c r="D90" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>210</v>
       </c>
       <c r="B91" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C91" t="s">
-        <v>26</v>
+        <v>5</v>
+      </c>
+      <c r="D91" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="B92" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C92" t="s">
-        <v>26</v>
+        <v>5</v>
+      </c>
+      <c r="D92" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="B93" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C93" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="B94" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C94" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="B95" t="s">
-        <v>211</v>
-      </c>
-      <c r="C95" t="s">
-        <v>30</v>
-      </c>
-      <c r="D95" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="B96" t="s">
-        <v>211</v>
-      </c>
-      <c r="C96" t="s">
-        <v>30</v>
-      </c>
-      <c r="D96" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B97" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C97" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B98" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C98" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B99" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C99" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D99" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="B100" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="B101" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>116</v>
+        <v>244</v>
       </c>
       <c r="B103" t="s">
-        <v>211</v>
-      </c>
-      <c r="C103" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>117</v>
+        <v>245</v>
       </c>
       <c r="B104" t="s">
-        <v>211</v>
-      </c>
-      <c r="C104" t="s">
-        <v>30</v>
-      </c>
-      <c r="D104" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>246</v>
       </c>
       <c r="B105" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C105" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D105" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>119</v>
+        <v>247</v>
       </c>
       <c r="B106" t="s">
-        <v>211</v>
-      </c>
-      <c r="C106" t="s">
-        <v>30</v>
-      </c>
-      <c r="D106" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>120</v>
+        <v>248</v>
       </c>
       <c r="B107" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C107" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D107" t="s">
-        <v>174</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>249</v>
       </c>
       <c r="B108" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C108" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D108" t="s">
-        <v>174</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>251</v>
       </c>
       <c r="B109" t="s">
-        <v>211</v>
-      </c>
-      <c r="C109" t="s">
-        <v>10</v>
-      </c>
-      <c r="D109" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>123</v>
+        <v>250</v>
       </c>
       <c r="B110" t="s">
-        <v>211</v>
-      </c>
-      <c r="C110" t="s">
-        <v>24</v>
-      </c>
-      <c r="D110" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="B111" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C111" t="s">
-        <v>24</v>
-      </c>
-      <c r="D111" t="s">
-        <v>174</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="B112" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C112" t="s">
-        <v>24</v>
-      </c>
-      <c r="D112" t="s">
-        <v>174</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="B113" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C113" t="s">
-        <v>41</v>
+        <v>12</v>
+      </c>
+      <c r="D113" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="B114" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C114" t="s">
-        <v>41</v>
+        <v>12</v>
+      </c>
+      <c r="D114" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B115" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C115" t="s">
+        <v>12</v>
+      </c>
+      <c r="D115" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="B116" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C116" t="s">
-        <v>73</v>
+        <v>12</v>
+      </c>
+      <c r="D116" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="B117" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C117" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D117" t="s">
-        <v>172</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="B118" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C118" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="B119" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C119" t="s">
+        <v>12</v>
+      </c>
+      <c r="D119" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="B120" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C120" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="B121" t="s">
-        <v>211</v>
-      </c>
-      <c r="C121" t="s">
-        <v>20</v>
-      </c>
-      <c r="D121" t="s">
-        <v>20</v>
+        <v>191</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="B122" t="s">
-        <v>211</v>
-      </c>
-      <c r="C122" t="s">
-        <v>136</v>
-      </c>
-      <c r="D122" t="s">
-        <v>136</v>
+        <v>191</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="B123" t="s">
-        <v>211</v>
-      </c>
-      <c r="C123" t="s">
-        <v>136</v>
-      </c>
-      <c r="D123" t="s">
-        <v>136</v>
+        <v>191</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="B124" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C124" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="B125" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="C125" t="s">
+        <v>12</v>
+      </c>
+      <c r="D125" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="B126" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C126" t="s">
-        <v>141</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="B127" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C127" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D127" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="B128" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>144</v>
+        <v>231</v>
       </c>
       <c r="B129" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>145</v>
+        <v>232</v>
       </c>
       <c r="B130" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>146</v>
+        <v>233</v>
       </c>
       <c r="B131" t="s">
-        <v>211</v>
-      </c>
-      <c r="C131" t="s">
-        <v>73</v>
+        <v>191</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>147</v>
+        <v>234</v>
       </c>
       <c r="B132" t="s">
-        <v>211</v>
-      </c>
-      <c r="C132" t="s">
-        <v>4</v>
-      </c>
-      <c r="D132" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="B133" t="s">
-        <v>211</v>
-      </c>
-      <c r="C133" t="s">
-        <v>26</v>
+        <v>191</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="B134" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C134" t="s">
-        <v>215</v>
+        <v>4</v>
+      </c>
+      <c r="D134" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="B135" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C135" t="s">
-        <v>215</v>
+        <v>4</v>
+      </c>
+      <c r="D135" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="B136" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C136" t="s">
-        <v>215</v>
+        <v>4</v>
+      </c>
+      <c r="D136" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="B137" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C137" t="s">
-        <v>215</v>
+        <v>10</v>
+      </c>
+      <c r="D137" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="B138" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C138" t="s">
-        <v>216</v>
+        <v>10</v>
+      </c>
+      <c r="D138" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>105</v>
+      </c>
+      <c r="B139" t="s">
+        <v>191</v>
+      </c>
+      <c r="C139" t="s">
+        <v>10</v>
+      </c>
+      <c r="D139" t="s">
         <v>154</v>
-      </c>
-      <c r="B139" t="s">
-        <v>211</v>
-      </c>
-      <c r="C139" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="B140" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C140" t="s">
-        <v>216</v>
+        <v>22</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="B141" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C141" t="s">
-        <v>216</v>
+        <v>22</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="B142" t="s">
-        <v>211</v>
-      </c>
-      <c r="C142" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="B143" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>159</v>
+        <v>237</v>
       </c>
       <c r="B144" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>160</v>
+        <v>109</v>
       </c>
       <c r="B145" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="C145" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>161</v>
+        <v>235</v>
       </c>
       <c r="B146" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>162</v>
+        <v>236</v>
       </c>
       <c r="B147" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
       <c r="B148" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="C148" t="s">
+        <v>1</v>
+      </c>
+      <c r="D148" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
       <c r="B149" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="J149" s="2"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>165</v>
+        <v>112</v>
       </c>
       <c r="B150" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="J150" s="2"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>166</v>
+        <v>113</v>
       </c>
       <c r="B151" t="s">
-        <v>211</v>
-      </c>
-      <c r="C151" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="J151" s="2"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>167</v>
+        <v>114</v>
       </c>
       <c r="B152" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C152" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D152" t="s">
+        <v>8</v>
+      </c>
+      <c r="J152" s="2"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="B153" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C153" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="D153" t="s">
+        <v>116</v>
+      </c>
+      <c r="J153" s="2"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="B154" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C154" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="D154" t="s">
+        <v>116</v>
+      </c>
+      <c r="J154" s="2"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="B155" t="s">
-        <v>211</v>
-      </c>
-      <c r="C155" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="J155" s="2"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="B156" t="s">
-        <v>211</v>
-      </c>
-      <c r="C156" t="s">
-        <v>220</v>
+        <v>191</v>
+      </c>
+      <c r="J156" s="2"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>120</v>
+      </c>
+      <c r="B157" t="s">
+        <v>191</v>
+      </c>
+      <c r="C157" t="s">
+        <v>121</v>
+      </c>
+      <c r="J157" s="2"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>122</v>
+      </c>
+      <c r="B158" t="s">
+        <v>191</v>
+      </c>
+      <c r="C158" t="s">
+        <v>9</v>
+      </c>
+      <c r="D158" t="s">
+        <v>9</v>
+      </c>
+      <c r="J158" s="2"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>123</v>
+      </c>
+      <c r="B159" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>124</v>
+      </c>
+      <c r="B160" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>125</v>
+      </c>
+      <c r="B161" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>126</v>
+      </c>
+      <c r="B162" t="s">
+        <v>191</v>
+      </c>
+      <c r="C162" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>127</v>
+      </c>
+      <c r="B163" t="s">
+        <v>191</v>
+      </c>
+      <c r="C163" t="s">
+        <v>252</v>
+      </c>
+      <c r="D163" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>128</v>
+      </c>
+      <c r="B164" t="s">
+        <v>191</v>
+      </c>
+      <c r="C164" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>130</v>
+      </c>
+      <c r="B165" t="s">
+        <v>191</v>
+      </c>
+      <c r="C165" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>131</v>
+      </c>
+      <c r="B166" t="s">
+        <v>191</v>
+      </c>
+      <c r="C166" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>129</v>
+      </c>
+      <c r="B167" t="s">
+        <v>191</v>
+      </c>
+      <c r="C167" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>132</v>
+      </c>
+      <c r="B168" t="s">
+        <v>191</v>
+      </c>
+      <c r="C168" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>134</v>
+      </c>
+      <c r="B169" t="s">
+        <v>191</v>
+      </c>
+      <c r="C169" t="s">
+        <v>196</v>
+      </c>
+      <c r="D169" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>135</v>
+      </c>
+      <c r="B170" t="s">
+        <v>191</v>
+      </c>
+      <c r="C170" t="s">
+        <v>196</v>
+      </c>
+      <c r="D170" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>136</v>
+      </c>
+      <c r="B171" t="s">
+        <v>191</v>
+      </c>
+      <c r="C171" t="s">
+        <v>196</v>
+      </c>
+      <c r="D171" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>133</v>
+      </c>
+      <c r="B172" t="s">
+        <v>191</v>
+      </c>
+      <c r="C172" t="s">
+        <v>196</v>
+      </c>
+      <c r="D172" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>137</v>
+      </c>
+      <c r="B173" t="s">
+        <v>191</v>
+      </c>
+      <c r="C173" t="s">
+        <v>196</v>
+      </c>
+      <c r="D173" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>138</v>
+      </c>
+      <c r="B174" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>140</v>
+      </c>
+      <c r="B175" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>139</v>
+      </c>
+      <c r="B176" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>141</v>
+      </c>
+      <c r="B177" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>142</v>
+      </c>
+      <c r="B178" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>143</v>
+      </c>
+      <c r="B179" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>144</v>
+      </c>
+      <c r="B180" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>145</v>
+      </c>
+      <c r="B181" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>147</v>
+      </c>
+      <c r="B182" t="s">
+        <v>191</v>
+      </c>
+      <c r="C182" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>148</v>
+      </c>
+      <c r="B183" t="s">
+        <v>191</v>
+      </c>
+      <c r="C183" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>149</v>
+      </c>
+      <c r="B184" t="s">
+        <v>191</v>
+      </c>
+      <c r="C184" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>146</v>
+      </c>
+      <c r="B185" t="s">
+        <v>191</v>
+      </c>
+      <c r="C185" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>150</v>
+      </c>
+      <c r="B186" t="s">
+        <v>191</v>
+      </c>
+      <c r="C186" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>151</v>
+      </c>
+      <c r="B187" t="s">
+        <v>191</v>
+      </c>
+      <c r="C187" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:A187">
+    <sortCondition ref="A2"/>
+  </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C174:C181 C188:C1048576">
       <formula1>all_tissues</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5180,298 +5594,298 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" t="s">
         <v>192</v>
       </c>
-      <c r="B11" t="s">
-        <v>212</v>
-      </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B21" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C22" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B27" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="B28" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5484,7 +5898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -5497,358 +5911,358 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" t="s">
         <v>192</v>
       </c>
-      <c r="B11" t="s">
-        <v>212</v>
-      </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C20" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="D20" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B21" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C22" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="D24" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C25" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="D25" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B27" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C27" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D27" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="B28" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5862,7 +6276,7 @@
   <dimension ref="A3:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B5" sqref="B5:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5873,184 +6287,184 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>